<commit_message>
Made Excel doc match example in paper.
</commit_message>
<xml_diff>
--- a/PLDI-2012/Monthly_Budget_Trunc.xlsx
+++ b/PLDI-2012/Monthly_Budget_Trunc.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="960" windowWidth="20355" windowHeight="9120"/>
+    <workbookView xWindow="22800" yWindow="10140" windowWidth="20360" windowHeight="9120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -24,9 +29,6 @@
     <t>Actual Cost</t>
   </si>
   <si>
-    <t>Mortgage or rent</t>
-  </si>
-  <si>
     <t>Phone</t>
   </si>
   <si>
@@ -54,7 +56,10 @@
     <t>Gasoline</t>
   </si>
   <si>
-    <t>Can I afford a fancy dinner?</t>
+    <t>Rent</t>
+  </si>
+  <si>
+    <t>Fancy dinner tonight?</t>
   </si>
 </sst>
 </file>
@@ -403,30 +408,30 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -436,9 +441,9 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>1150</v>
@@ -448,9 +453,9 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>3675</v>
@@ -460,9 +465,9 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>80</v>
@@ -472,9 +477,9 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>11.25</v>
@@ -484,9 +489,9 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>200</v>
@@ -496,9 +501,9 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>225</v>
@@ -508,9 +513,9 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>50</v>
@@ -520,9 +525,9 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1">
         <v>100</v>
@@ -532,9 +537,9 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1">
         <f>SUM(B3:B10)</f>
@@ -546,7 +551,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -559,6 +564,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -568,13 +578,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -584,12 +599,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>